<commit_message>
added data into datasets+ tweaked the code a lil more
</commit_message>
<xml_diff>
--- a/updated_trades.xlsx
+++ b/updated_trades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -37,6 +37,33 @@
     <t>Accumulated Profit/Loss</t>
   </si>
   <si>
+    <t>GDHG</t>
+  </si>
+  <si>
+    <t>LPTV</t>
+  </si>
+  <si>
+    <t>SNTI</t>
+  </si>
+  <si>
+    <t>LUCY</t>
+  </si>
+  <si>
+    <t>GOVX</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>OPTT</t>
+  </si>
+  <si>
+    <t>MBIO</t>
+  </si>
+  <si>
+    <t>ANVS</t>
+  </si>
+  <si>
     <t>KOSS</t>
   </si>
   <si>
@@ -50,9 +77,6 @@
   </si>
   <si>
     <t>CIFR</t>
-  </si>
-  <si>
-    <t>TSLA</t>
   </si>
   <si>
     <t>ZAPP</t>
@@ -471,7 +495,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -511,156 +535,386 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5">
-        <v>25569.313026342592</v>
+        <v>25569.313026319443</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="7">
-        <v>5.94</v>
+        <v>0.1895</v>
       </c>
       <c r="D2" s="7">
-        <v>6.35</v>
+        <v>0.178</v>
       </c>
       <c r="E2" s="8">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="F2" s="7">
-        <v>0.9099999999999966</v>
+        <v>-6.890000000000001</v>
       </c>
       <c r="G2" s="7">
-        <v>0.9099999999999966</v>
+        <v>-6.890000000000001</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5">
-        <v>25569.313026342592</v>
+        <v>25569.313026319443</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="7">
-        <v>3.15</v>
+        <v>0.1506</v>
       </c>
       <c r="D3" s="7">
-        <v>2.69</v>
+        <v>0.14</v>
       </c>
       <c r="E3" s="8">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="F3" s="7">
-        <v>-5.739999999999998</v>
+        <v>-6.440000000000012</v>
       </c>
       <c r="G3" s="7">
-        <v>-4.830000000000002</v>
+        <v>-13.33000000000001</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5">
-        <v>25569.313026342592</v>
+        <v>25569.313026319443</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="7">
-        <v>0.2165</v>
+        <v>0.4851</v>
       </c>
       <c r="D4" s="7">
-        <v>0.206</v>
+        <v>0.52</v>
       </c>
       <c r="E4" s="8">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F4" s="7">
-        <v>-3.240000000000002</v>
+        <v>16.31000000000003</v>
       </c>
       <c r="G4" s="7">
-        <v>-8.070000000000004</v>
+        <v>2.980000000000018</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5">
-        <v>25569.313026342592</v>
+        <v>25569.313026319443</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="7">
-        <v>2.8</v>
+        <v>0.47</v>
       </c>
       <c r="D5" s="7">
-        <v>2.28</v>
+        <v>0.52</v>
       </c>
       <c r="E5" s="8">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="F5" s="7">
-        <v>-53.14000000000004</v>
+        <v>18.85999999999999</v>
       </c>
       <c r="G5" s="7">
-        <v>-61.21000000000005</v>
+        <v>21.84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5">
-        <v>25569.313026342592</v>
+        <v>25569.313026319443</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="7">
-        <v>4.79</v>
+        <v>0.5165</v>
       </c>
       <c r="D6" s="7">
-        <v>4.67</v>
+        <v>0.4921</v>
       </c>
       <c r="E6" s="8">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="F6" s="7">
-        <v>-13.13999999999999</v>
+        <v>-13.34000000000003</v>
       </c>
       <c r="G6" s="7">
-        <v>-74.35000000000004</v>
+        <v>8.499999999999972</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5">
-        <v>25569.313026342592</v>
+        <v>25569.313026319443</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="7">
-        <v>247.19</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>3.61</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3.55</v>
+      </c>
       <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="F7" s="7">
+        <v>-5.04000000000002</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3.459999999999951</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5">
+        <v>25569.31302633102</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="7">
+        <v>210.82</v>
+      </c>
+      <c r="D8" s="7">
+        <v>226.46</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>30.14000000000004</v>
+      </c>
+      <c r="G8" s="7">
+        <v>30.14000000000004</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="5">
+        <v>25569.31302633102</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.455</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.54</v>
+      </c>
+      <c r="E9" s="8">
+        <v>100</v>
+      </c>
+      <c r="F9" s="7">
+        <v>7.359999999999999</v>
+      </c>
+      <c r="G9" s="7">
+        <v>37.50000000000004</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="5">
+        <v>25569.31302633102</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.535</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.566</v>
+      </c>
+      <c r="E10" s="8">
+        <v>100</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1.959999999999994</v>
+      </c>
+      <c r="G10" s="7">
+        <v>39.46000000000004</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="5">
+        <v>25569.31302633102</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6.47</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10.71</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3.100000000000001</v>
+      </c>
+      <c r="G11" s="7">
+        <v>42.56000000000004</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="5">
         <v>25569.313026342592</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7">
+        <v>5.94</v>
+      </c>
+      <c r="D12" s="7">
+        <v>6.35</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.9099999999999966</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.9099999999999966</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="5">
+        <v>25569.313026342592</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3.15</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2.69</v>
+      </c>
+      <c r="E13" s="8">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7">
+        <v>-5.739999999999998</v>
+      </c>
+      <c r="G13" s="7">
+        <v>-4.830000000000002</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="5">
+        <v>25569.313026342592</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.2165</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.206</v>
+      </c>
+      <c r="E14" s="8">
+        <v>200</v>
+      </c>
+      <c r="F14" s="7">
+        <v>-3.240000000000002</v>
+      </c>
+      <c r="G14" s="7">
+        <v>-8.070000000000004</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="5">
+        <v>25569.313026342592</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2.28</v>
+      </c>
+      <c r="E15" s="8">
+        <v>100</v>
+      </c>
+      <c r="F15" s="7">
+        <v>-53.14000000000004</v>
+      </c>
+      <c r="G15" s="7">
+        <v>-61.21000000000005</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="5">
+        <v>25569.313026342592</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4.79</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4.67</v>
+      </c>
+      <c r="E16" s="8">
+        <v>100</v>
+      </c>
+      <c r="F16" s="7">
+        <v>-13.13999999999999</v>
+      </c>
+      <c r="G16" s="7">
+        <v>-74.35000000000004</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="5">
+        <v>25569.313026342592</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="7">
+        <v>247.19</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="5">
+        <v>25569.313026342592</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="7">
         <v>2.93</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D18" s="7">
         <v>3.15</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E18" s="8">
         <v>156</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F18" s="7">
         <v>33.17999999999995</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G18" s="7">
         <v>-41.17000000000009</v>
       </c>
     </row>

</xml_diff>